<commit_message>
finishing icp limits and report section
</commit_message>
<xml_diff>
--- a/application/example2.xlsx
+++ b/application/example2.xlsx
@@ -87,9 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -98,7 +101,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -473,7 +476,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,6 +485,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="19" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1" ht="13" customHeight="1">
@@ -500,7 +504,11 @@
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>W171981</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="13" customHeight="1">
       <c r="A2" s="1" t="inlineStr">
@@ -609,7 +617,7 @@
       <c r="H8" s="1" t="n"/>
     </row>
     <row r="9" ht="13" customHeight="1">
-      <c r="A9" s="2" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">Samples:  1) STBD Tank 03Jan23 12:07p  2) Galley 03Jan23 12:30p  3) After Filter 03Jan23 12:21p  4) Z01 03Jan23 12:30p </t>
         </is>
@@ -622,17 +630,17 @@
       <c r="G9" s="1" t="n"/>
       <c r="H9" s="1" t="n"/>
     </row>
-    <row r="10">
-      <c r="A10" s="3" t="n"/>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n"/>
-      <c r="D10" s="3" t="n"/>
-      <c r="E10" s="3" t="n"/>
-      <c r="F10" s="3" t="n"/>
-      <c r="G10" s="3" t="n"/>
-      <c r="H10" s="3" t="n"/>
-    </row>
-    <row r="11">
+    <row r="10" ht="13" customHeight="1">
+      <c r="A10" s="4" t="n"/>
+      <c r="B10" s="4" t="n"/>
+      <c r="C10" s="4" t="n"/>
+      <c r="D10" s="4" t="n"/>
+      <c r="E10" s="4" t="n"/>
+      <c r="F10" s="4" t="n"/>
+      <c r="G10" s="4" t="n"/>
+      <c r="H10" s="4" t="n"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="n"/>
       <c r="C11" s="1" t="n"/>
@@ -642,1127 +650,1363 @@
       <c r="G11" s="1" t="n"/>
       <c r="H11" s="1" t="n"/>
     </row>
-    <row r="12">
+    <row r="12" ht="13" customHeight="1">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Tests</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
+          <t>Elements</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>Symbols</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Sample 1</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>Sample 2</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>Sample 3</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>Sample 4</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr">
-        <is>
-          <t>Sample 1</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="inlineStr">
-        <is>
-          <t>Sample 2</t>
-        </is>
-      </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>Sample 3</t>
-        </is>
-      </c>
-      <c r="F12" s="4" t="inlineStr">
-        <is>
-          <t>Sample 4</t>
-        </is>
-      </c>
-      <c r="G12" s="4" t="inlineStr">
-        <is>
-          <t>So</t>
-        </is>
-      </c>
-      <c r="H12" s="5" t="inlineStr">
-        <is>
-          <t>Ref Value</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="7" t="n"/>
-      <c r="C13" s="7" t="n"/>
-      <c r="D13" s="7" t="n"/>
-      <c r="E13" s="7" t="n"/>
-      <c r="F13" s="7" t="n"/>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="7" t="n"/>
+      <c r="H12" s="6" t="inlineStr">
+        <is>
+          <t>Maximum Limits</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="7" t="n"/>
+      <c r="B13" s="8" t="n"/>
+      <c r="C13" s="8" t="n"/>
+      <c r="D13" s="8" t="n"/>
+      <c r="E13" s="8" t="n"/>
+      <c r="F13" s="8" t="n"/>
+      <c r="G13" s="8" t="n"/>
+      <c r="H13" s="8" t="n"/>
     </row>
     <row r="14" ht="13" customHeight="1">
-      <c r="A14" s="8" t="inlineStr">
+      <c r="A14" s="9" t="inlineStr">
         <is>
           <t>1) Aluminium</t>
         </is>
       </c>
-      <c r="B14" s="9" t="inlineStr">
+      <c r="B14" s="10" t="inlineStr">
         <is>
           <t>Al</t>
         </is>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="10" t="n">
         <v>0.108</v>
       </c>
-      <c r="D14" s="9" t="n">
+      <c r="D14" s="10" t="n">
         <v>0.146</v>
       </c>
-      <c r="E14" s="9" t="n">
+      <c r="E14" s="10" t="n">
         <v>0.135</v>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="10" t="n">
         <v>0.145</v>
       </c>
-      <c r="G14" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H14" s="1" t="n"/>
+      <c r="G14" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H14" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="13" customHeight="1">
-      <c r="A15" s="8" t="inlineStr">
+      <c r="A15" s="9" t="inlineStr">
         <is>
           <t>2) Antimony</t>
         </is>
       </c>
-      <c r="B15" s="9" t="inlineStr">
+      <c r="B15" s="10" t="inlineStr">
         <is>
           <t>Sb</t>
         </is>
       </c>
-      <c r="C15" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="D15" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="E15" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="F15" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="G15" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H15" s="1" t="n"/>
+      <c r="C15" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D15" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F15" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G15" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H15" s="6" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="13" customHeight="1">
-      <c r="A16" s="8" t="inlineStr">
+      <c r="A16" s="9" t="inlineStr">
         <is>
           <t>3) Arsenic</t>
         </is>
       </c>
-      <c r="B16" s="9" t="inlineStr">
+      <c r="B16" s="10" t="inlineStr">
         <is>
           <t>As</t>
         </is>
       </c>
-      <c r="C16" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="D16" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="E16" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="F16" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="G16" s="9" t="inlineStr">
+      <c r="C16" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F16" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G16" s="10" t="inlineStr">
         <is>
           <t>ug/L</t>
         </is>
       </c>
-      <c r="H16" s="1" t="n"/>
+      <c r="H16" s="6" t="inlineStr">
+        <is>
+          <t>10.0mg/L</t>
+        </is>
+      </c>
     </row>
     <row r="17" ht="13" customHeight="1">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="A17" s="9" t="inlineStr">
         <is>
           <t>4) Barium</t>
         </is>
       </c>
-      <c r="B17" s="9" t="inlineStr">
+      <c r="B17" s="10" t="inlineStr">
         <is>
           <t>Ba</t>
         </is>
       </c>
-      <c r="C17" s="9" t="n">
-        <v>0.0045</v>
-      </c>
-      <c r="D17" s="9" t="n">
-        <v>0.0047</v>
-      </c>
-      <c r="E17" s="9" t="n">
-        <v>0.0041</v>
-      </c>
-      <c r="F17" s="9" t="n">
-        <v>0.0039</v>
-      </c>
-      <c r="G17" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H17" s="1" t="n"/>
+      <c r="C17" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 0.009</t>
+        </is>
+      </c>
+      <c r="D17" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 0.009</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 0.009</t>
+        </is>
+      </c>
+      <c r="F17" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 0.009</t>
+        </is>
+      </c>
+      <c r="G17" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H17" s="6" t="inlineStr">
+        <is>
+          <t>2.0mg/L</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="13" customHeight="1">
-      <c r="A18" s="8" t="inlineStr">
+      <c r="A18" s="9" t="inlineStr">
         <is>
           <t>5) Beryllium</t>
         </is>
       </c>
-      <c r="B18" s="9" t="inlineStr">
+      <c r="B18" s="10" t="inlineStr">
         <is>
           <t>Be</t>
         </is>
       </c>
-      <c r="C18" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H18" s="1" t="n"/>
+      <c r="C18" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="D18" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="F18" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="G18" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H18" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="13" customHeight="1">
-      <c r="A19" s="8" t="inlineStr">
+      <c r="A19" s="9" t="inlineStr">
         <is>
           <t>6) Boron</t>
         </is>
       </c>
-      <c r="B19" s="9" t="inlineStr">
+      <c r="B19" s="10" t="inlineStr">
         <is>
           <t>B</t>
         </is>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="10" t="n">
         <v>0.422</v>
       </c>
-      <c r="D19" s="9" t="n">
+      <c r="D19" s="10" t="n">
         <v>0.499</v>
       </c>
-      <c r="E19" s="9" t="n">
+      <c r="E19" s="10" t="n">
         <v>0.493</v>
       </c>
-      <c r="F19" s="9" t="n">
+      <c r="F19" s="10" t="n">
         <v>0.51</v>
       </c>
-      <c r="G19" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H19" s="1" t="n"/>
+      <c r="G19" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H19" s="6" t="inlineStr">
+        <is>
+          <t>5.0mg/L</t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="13" customHeight="1">
-      <c r="A20" s="8" t="inlineStr">
+      <c r="A20" s="9" t="inlineStr">
         <is>
           <t>7) Cadmium</t>
         </is>
       </c>
-      <c r="B20" s="9" t="inlineStr">
+      <c r="B20" s="10" t="inlineStr">
         <is>
           <t>Cd</t>
         </is>
       </c>
-      <c r="C20" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="D20" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="E20" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="F20" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="G20" s="9" t="inlineStr">
+      <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D20" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F20" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G20" s="10" t="inlineStr">
         <is>
           <t>ug/L</t>
         </is>
       </c>
-      <c r="H20" s="1" t="n"/>
+      <c r="H20" s="6" t="inlineStr">
+        <is>
+          <t>7.0mg/L</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="13" customHeight="1">
-      <c r="A21" s="8" t="inlineStr">
+      <c r="A21" s="9" t="inlineStr">
         <is>
           <t>8) Calcium</t>
         </is>
       </c>
-      <c r="B21" s="9" t="inlineStr">
+      <c r="B21" s="10" t="inlineStr">
         <is>
           <t>Ca</t>
         </is>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="10" t="n">
         <v>7.18</v>
       </c>
-      <c r="D21" s="9" t="n">
+      <c r="D21" s="10" t="n">
         <v>7.1</v>
       </c>
-      <c r="E21" s="9" t="n">
+      <c r="E21" s="10" t="n">
         <v>6.82</v>
       </c>
-      <c r="F21" s="9" t="n">
+      <c r="F21" s="10" t="n">
         <v>6.24</v>
       </c>
-      <c r="G21" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H21" s="1" t="n"/>
+      <c r="G21" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H21" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Testing out this comment </t>
+        </is>
+      </c>
     </row>
     <row r="22" ht="13" customHeight="1">
-      <c r="A22" s="8" t="inlineStr">
+      <c r="A22" s="9" t="inlineStr">
         <is>
           <t>9) Chromium</t>
         </is>
       </c>
-      <c r="B22" s="9" t="inlineStr">
+      <c r="B22" s="10" t="inlineStr">
         <is>
           <t>Cr</t>
         </is>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="10" t="n">
         <v>0.0002</v>
       </c>
-      <c r="D22" s="9" t="n">
+      <c r="D22" s="10" t="n">
         <v>0.0002</v>
       </c>
-      <c r="E22" s="9" t="n">
+      <c r="E22" s="10" t="n">
         <v>0.0004</v>
       </c>
-      <c r="F22" s="9" t="n">
+      <c r="F22" s="10" t="n">
         <v>0.0005</v>
       </c>
-      <c r="G22" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="n"/>
+      <c r="G22" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H22" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="23" ht="13" customHeight="1">
-      <c r="A23" s="8" t="inlineStr">
+      <c r="A23" s="9" t="inlineStr">
         <is>
           <t>10) Cobalt</t>
         </is>
       </c>
-      <c r="B23" s="9" t="inlineStr">
+      <c r="B23" s="10" t="inlineStr">
         <is>
           <t>Co</t>
         </is>
       </c>
-      <c r="C23" s="9" t="inlineStr">
+      <c r="C23" s="10" t="inlineStr">
         <is>
           <t>&lt; 0.005</t>
         </is>
       </c>
-      <c r="D23" s="9" t="inlineStr">
+      <c r="D23" s="10" t="inlineStr">
         <is>
           <t>&lt; 0.005</t>
         </is>
       </c>
-      <c r="E23" s="9" t="inlineStr">
+      <c r="E23" s="10" t="inlineStr">
         <is>
           <t>&lt; 0.005</t>
         </is>
       </c>
-      <c r="F23" s="9" t="inlineStr">
+      <c r="F23" s="10" t="inlineStr">
         <is>
           <t>&lt; 0.005</t>
         </is>
       </c>
-      <c r="G23" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H23" s="1" t="n"/>
+      <c r="G23" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H23" s="6" t="inlineStr">
+        <is>
+          <t>100.0mg/L</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="13" customHeight="1">
-      <c r="A24" s="8" t="inlineStr">
+      <c r="A24" s="9" t="inlineStr">
         <is>
           <t>11) Copper</t>
         </is>
       </c>
-      <c r="B24" s="9" t="inlineStr">
+      <c r="B24" s="10" t="inlineStr">
         <is>
           <t>Cu</t>
         </is>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="D24" s="9" t="n">
+      <c r="D24" s="10" t="n">
         <v>0.042</v>
       </c>
-      <c r="E24" s="9" t="n">
+      <c r="E24" s="10" t="n">
         <v>0.039</v>
       </c>
-      <c r="F24" s="9" t="n">
+      <c r="F24" s="10" t="n">
         <v>0.039</v>
       </c>
-      <c r="G24" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H24" s="1" t="n"/>
+      <c r="G24" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H24" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="13" customHeight="1">
-      <c r="A25" s="8" t="inlineStr">
+      <c r="A25" s="9" t="inlineStr">
         <is>
           <t>12) Gold</t>
         </is>
       </c>
-      <c r="B25" s="9" t="inlineStr">
+      <c r="B25" s="10" t="inlineStr">
         <is>
           <t>Au</t>
         </is>
       </c>
-      <c r="C25" s="9" t="inlineStr">
+      <c r="C25" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="D25" s="9" t="inlineStr">
+      <c r="D25" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="E25" s="9" t="inlineStr">
+      <c r="E25" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="F25" s="9" t="inlineStr">
+      <c r="F25" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="G25" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H25" s="1" t="n"/>
+      <c r="G25" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H25" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="13" customHeight="1">
-      <c r="A26" s="8" t="inlineStr">
+      <c r="A26" s="9" t="inlineStr">
         <is>
           <t>13) Iron</t>
         </is>
       </c>
-      <c r="B26" s="9" t="inlineStr">
+      <c r="B26" s="10" t="inlineStr">
         <is>
           <t>Fe</t>
         </is>
       </c>
-      <c r="C26" s="9" t="n">
+      <c r="C26" s="10" t="n">
         <v>0.207</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="10" t="n">
         <v>0.193</v>
       </c>
-      <c r="E26" s="9" t="n">
+      <c r="E26" s="10" t="n">
         <v>0.098</v>
       </c>
-      <c r="F26" s="9" t="n">
+      <c r="F26" s="10" t="n">
         <v>0.267</v>
       </c>
-      <c r="G26" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H26" s="1" t="n"/>
+      <c r="G26" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H26" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="27" ht="13" customHeight="1">
-      <c r="A27" s="8" t="inlineStr">
+      <c r="A27" s="9" t="inlineStr">
         <is>
           <t>14) Lanthanum</t>
         </is>
       </c>
-      <c r="B27" s="9" t="inlineStr">
+      <c r="B27" s="10" t="inlineStr">
         <is>
           <t>La</t>
         </is>
       </c>
-      <c r="C27" s="9" t="inlineStr">
+      <c r="C27" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="D27" s="9" t="inlineStr">
+      <c r="D27" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="E27" s="9" t="inlineStr">
+      <c r="E27" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="F27" s="9" t="inlineStr">
+      <c r="F27" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="G27" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H27" s="1" t="n"/>
+      <c r="G27" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H27" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="13" customHeight="1">
-      <c r="A28" s="8" t="inlineStr">
+      <c r="A28" s="9" t="inlineStr">
         <is>
           <t>15) Lead</t>
         </is>
       </c>
-      <c r="B28" s="9" t="inlineStr">
+      <c r="B28" s="10" t="inlineStr">
         <is>
           <t>Pb</t>
         </is>
       </c>
-      <c r="C28" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="D28" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="E28" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="F28" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="G28" s="9" t="inlineStr">
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D28" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F28" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G28" s="10" t="inlineStr">
         <is>
           <t>ug/L</t>
         </is>
       </c>
-      <c r="H28" s="1" t="n"/>
+      <c r="H28" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="13" customHeight="1">
-      <c r="A29" s="8" t="inlineStr">
+      <c r="A29" s="9" t="inlineStr">
         <is>
           <t>16) Magnesium</t>
         </is>
       </c>
-      <c r="B29" s="9" t="inlineStr">
+      <c r="B29" s="10" t="inlineStr">
         <is>
           <t>Mg</t>
         </is>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="10" t="n">
         <v>1.32</v>
       </c>
-      <c r="D29" s="9" t="n">
+      <c r="D29" s="10" t="n">
         <v>1.3</v>
       </c>
-      <c r="E29" s="9" t="n">
+      <c r="E29" s="10" t="n">
         <v>1.25</v>
       </c>
-      <c r="F29" s="9" t="n">
+      <c r="F29" s="10" t="n">
         <v>1.14</v>
       </c>
-      <c r="G29" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H29" s="1" t="n"/>
+      <c r="G29" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H29" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="13" customHeight="1">
-      <c r="A30" s="8" t="inlineStr">
+      <c r="A30" s="9" t="inlineStr">
         <is>
           <t>17) Manganese</t>
         </is>
       </c>
-      <c r="B30" s="9" t="inlineStr">
+      <c r="B30" s="10" t="inlineStr">
         <is>
           <t>Mn</t>
         </is>
       </c>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="10" t="n">
         <v>0.005</v>
       </c>
-      <c r="D30" s="9" t="n">
+      <c r="D30" s="10" t="n">
         <v>0.005</v>
       </c>
-      <c r="E30" s="9" t="n">
+      <c r="E30" s="10" t="n">
         <v>0.004</v>
       </c>
-      <c r="F30" s="9" t="n">
+      <c r="F30" s="10" t="n">
         <v>0.005</v>
       </c>
-      <c r="G30" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H30" s="1" t="n"/>
+      <c r="G30" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H30" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="13" customHeight="1">
-      <c r="A31" s="8" t="inlineStr">
+      <c r="A31" s="9" t="inlineStr">
         <is>
           <t>18) Mercury</t>
         </is>
       </c>
-      <c r="B31" s="9" t="inlineStr">
+      <c r="B31" s="10" t="inlineStr">
         <is>
           <t>Hg</t>
         </is>
       </c>
-      <c r="C31" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="D31" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="E31" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="F31" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="G31" s="9" t="inlineStr">
+      <c r="C31" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D31" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E31" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F31" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G31" s="10" t="inlineStr">
         <is>
           <t>ug/L</t>
         </is>
       </c>
-      <c r="H31" s="1" t="n"/>
+      <c r="H31" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="32" ht="13" customHeight="1">
-      <c r="A32" s="8" t="inlineStr">
+      <c r="A32" s="9" t="inlineStr">
         <is>
           <t>19) Molybdenum</t>
         </is>
       </c>
-      <c r="B32" s="9" t="inlineStr">
+      <c r="B32" s="10" t="inlineStr">
         <is>
           <t>Mo</t>
         </is>
       </c>
-      <c r="C32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H32" s="1" t="n"/>
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="D32" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="E32" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="F32" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="G32" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H32" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="13" customHeight="1">
-      <c r="A33" s="8" t="inlineStr">
+      <c r="A33" s="9" t="inlineStr">
         <is>
           <t>20) Nickel</t>
         </is>
       </c>
-      <c r="B33" s="9" t="inlineStr">
+      <c r="B33" s="10" t="inlineStr">
         <is>
           <t>Ni</t>
         </is>
       </c>
-      <c r="C33" s="9" t="n">
+      <c r="C33" s="10" t="n">
         <v>0.003</v>
       </c>
-      <c r="D33" s="9" t="n">
+      <c r="D33" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="E33" s="9" t="n">
+      <c r="E33" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="F33" s="9" t="n">
+      <c r="F33" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="G33" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H33" s="1" t="n"/>
+      <c r="G33" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H33" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="13" customHeight="1">
-      <c r="A34" s="8" t="inlineStr">
+      <c r="A34" s="9" t="inlineStr">
         <is>
           <t>21) Phosphorus</t>
         </is>
       </c>
-      <c r="B34" s="9" t="inlineStr">
+      <c r="B34" s="10" t="inlineStr">
         <is>
           <t>P</t>
         </is>
       </c>
-      <c r="C34" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="9" t="n">
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="D34" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="E34" s="9" t="n">
+      <c r="E34" s="10" t="n">
         <v>-0.003</v>
       </c>
-      <c r="F34" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G34" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H34" s="1" t="n"/>
+      <c r="F34" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="G34" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H34" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="13" customHeight="1">
-      <c r="A35" s="8" t="inlineStr">
+      <c r="A35" s="9" t="inlineStr">
         <is>
           <t>22) Potassium</t>
         </is>
       </c>
-      <c r="B35" s="9" t="inlineStr">
+      <c r="B35" s="10" t="inlineStr">
         <is>
           <t>K</t>
         </is>
       </c>
-      <c r="C35" s="9" t="n">
+      <c r="C35" s="10" t="n">
         <v>0.13</v>
       </c>
-      <c r="D35" s="9" t="n">
+      <c r="D35" s="10" t="n">
         <v>0.15</v>
       </c>
-      <c r="E35" s="9" t="n">
+      <c r="E35" s="10" t="n">
         <v>0.14</v>
       </c>
-      <c r="F35" s="9" t="n">
+      <c r="F35" s="10" t="n">
         <v>0.13</v>
       </c>
-      <c r="G35" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H35" s="1" t="n"/>
+      <c r="G35" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H35" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="13" customHeight="1">
-      <c r="A36" s="8" t="inlineStr">
+      <c r="A36" s="9" t="inlineStr">
         <is>
           <t>23) Scandium</t>
         </is>
       </c>
-      <c r="B36" s="9" t="inlineStr">
+      <c r="B36" s="10" t="inlineStr">
         <is>
           <t>Sc</t>
         </is>
       </c>
-      <c r="C36" s="9" t="inlineStr">
+      <c r="C36" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="D36" s="9" t="inlineStr">
+      <c r="D36" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="E36" s="9" t="inlineStr">
+      <c r="E36" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="F36" s="9" t="inlineStr">
+      <c r="F36" s="10" t="inlineStr">
         <is>
           <t>n/a</t>
         </is>
       </c>
-      <c r="G36" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H36" s="1" t="n"/>
+      <c r="G36" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H36" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="13" customHeight="1">
-      <c r="A37" s="8" t="inlineStr">
+      <c r="A37" s="9" t="inlineStr">
         <is>
           <t>24) Selenium</t>
         </is>
       </c>
-      <c r="B37" s="9" t="inlineStr">
+      <c r="B37" s="10" t="inlineStr">
         <is>
           <t>Se</t>
         </is>
       </c>
-      <c r="C37" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="D37" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="E37" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="F37" s="9" t="inlineStr">
-        <is>
-          <t>ND</t>
-        </is>
-      </c>
-      <c r="G37" s="9" t="inlineStr">
+      <c r="C37" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D37" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E37" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F37" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G37" s="10" t="inlineStr">
         <is>
           <t>ug/L</t>
         </is>
       </c>
-      <c r="H37" s="1" t="n"/>
+      <c r="H37" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="13" customHeight="1">
-      <c r="A38" s="8" t="inlineStr">
+      <c r="A38" s="9" t="inlineStr">
         <is>
           <t>25) Silicon</t>
         </is>
       </c>
-      <c r="B38" s="9" t="inlineStr">
+      <c r="B38" s="10" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
       </c>
-      <c r="C38" s="9" t="n">
+      <c r="C38" s="10" t="n">
         <v>2.34</v>
       </c>
-      <c r="D38" s="9" t="n">
+      <c r="D38" s="10" t="n">
         <v>2.4</v>
       </c>
-      <c r="E38" s="9" t="n">
+      <c r="E38" s="10" t="n">
         <v>2.31</v>
       </c>
-      <c r="F38" s="9" t="n">
+      <c r="F38" s="10" t="n">
         <v>2.17</v>
       </c>
-      <c r="G38" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H38" s="1" t="n"/>
+      <c r="G38" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H38" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="13" customHeight="1">
-      <c r="A39" s="8" t="inlineStr">
+      <c r="A39" s="9" t="inlineStr">
         <is>
           <t>26) Silver</t>
         </is>
       </c>
-      <c r="B39" s="9" t="inlineStr">
+      <c r="B39" s="10" t="inlineStr">
         <is>
           <t>Ag</t>
         </is>
       </c>
-      <c r="C39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H39" s="1" t="n"/>
+      <c r="C39" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="D39" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="E39" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="F39" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="G39" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H39" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="40" ht="13" customHeight="1">
-      <c r="A40" s="8" t="inlineStr">
+      <c r="A40" s="9" t="inlineStr">
         <is>
           <t>27) Sodium</t>
         </is>
       </c>
-      <c r="B40" s="9" t="inlineStr">
+      <c r="B40" s="10" t="inlineStr">
         <is>
           <t>Na</t>
         </is>
       </c>
-      <c r="C40" s="9" t="n">
+      <c r="C40" s="10" t="n">
         <v>3.68</v>
       </c>
-      <c r="D40" s="9" t="n">
+      <c r="D40" s="10" t="n">
         <v>3.58</v>
       </c>
-      <c r="E40" s="9" t="n">
+      <c r="E40" s="10" t="n">
         <v>3.5</v>
       </c>
-      <c r="F40" s="9" t="n">
+      <c r="F40" s="10" t="n">
         <v>3.21</v>
       </c>
-      <c r="G40" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H40" s="1" t="n"/>
+      <c r="G40" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H40" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="13" customHeight="1">
-      <c r="A41" s="8" t="inlineStr">
+      <c r="A41" s="9" t="inlineStr">
         <is>
           <t>28) Strontium</t>
         </is>
       </c>
-      <c r="B41" s="9" t="inlineStr">
+      <c r="B41" s="10" t="inlineStr">
         <is>
           <t>Sr</t>
         </is>
       </c>
-      <c r="C41" s="9" t="n">
+      <c r="C41" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="D41" s="9" t="n">
+      <c r="D41" s="10" t="n">
         <v>0.02</v>
       </c>
-      <c r="E41" s="9" t="n">
+      <c r="E41" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="F41" s="9" t="n">
+      <c r="F41" s="10" t="n">
         <v>0.01</v>
       </c>
-      <c r="G41" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H41" s="1" t="n"/>
+      <c r="G41" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H41" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="42" ht="13" customHeight="1">
-      <c r="A42" s="8" t="inlineStr">
+      <c r="A42" s="9" t="inlineStr">
         <is>
           <t>29) Tin</t>
         </is>
       </c>
-      <c r="B42" s="9" t="inlineStr">
+      <c r="B42" s="10" t="inlineStr">
         <is>
           <t>Sn</t>
         </is>
       </c>
-      <c r="C42" s="9" t="n">
+      <c r="C42" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="D42" s="9" t="n">
+      <c r="D42" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="E42" s="9" t="n">
+      <c r="E42" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="F42" s="9" t="n">
+      <c r="F42" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="G42" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H42" s="1" t="n"/>
+      <c r="G42" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H42" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="43" ht="13" customHeight="1">
-      <c r="A43" s="8" t="inlineStr">
+      <c r="A43" s="9" t="inlineStr">
         <is>
           <t>30) Titanium</t>
         </is>
       </c>
-      <c r="B43" s="9" t="inlineStr">
+      <c r="B43" s="10" t="inlineStr">
         <is>
           <t>Ti</t>
         </is>
       </c>
-      <c r="C43" s="9" t="n">
+      <c r="C43" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="D43" s="9" t="n">
+      <c r="D43" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="E43" s="9" t="n">
+      <c r="E43" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="F43" s="9" t="n">
+      <c r="F43" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="G43" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H43" s="1" t="n"/>
+      <c r="G43" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H43" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="44" ht="13" customHeight="1">
-      <c r="A44" s="8" t="inlineStr">
+      <c r="A44" s="9" t="inlineStr">
         <is>
           <t>31) Tungsten</t>
         </is>
       </c>
-      <c r="B44" s="9" t="inlineStr">
+      <c r="B44" s="10" t="inlineStr">
         <is>
           <t>W</t>
         </is>
       </c>
-      <c r="C44" s="9" t="n">
+      <c r="C44" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="D44" s="9" t="n">
+      <c r="D44" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="E44" s="9" t="n">
+      <c r="E44" s="10" t="n">
         <v>0.002</v>
       </c>
-      <c r="F44" s="9" t="n">
+      <c r="F44" s="10" t="n">
         <v>0.001</v>
       </c>
-      <c r="G44" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H44" s="1" t="n"/>
+      <c r="G44" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H44" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="45" ht="13" customHeight="1">
-      <c r="A45" s="8" t="inlineStr">
+      <c r="A45" s="9" t="inlineStr">
         <is>
           <t>32) Vanadium</t>
         </is>
       </c>
-      <c r="B45" s="9" t="inlineStr">
+      <c r="B45" s="10" t="inlineStr">
         <is>
           <t>V</t>
         </is>
       </c>
-      <c r="C45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H45" s="1" t="n"/>
+      <c r="C45" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="D45" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="E45" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="F45" s="10" t="inlineStr">
+        <is>
+          <t>ND2</t>
+        </is>
+      </c>
+      <c r="G45" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H45" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
     <row r="46" ht="13" customHeight="1">
-      <c r="A46" s="8" t="inlineStr">
+      <c r="A46" s="9" t="inlineStr">
         <is>
           <t>33) Zinc</t>
         </is>
       </c>
-      <c r="B46" s="9" t="inlineStr">
+      <c r="B46" s="10" t="inlineStr">
         <is>
           <t>Zn</t>
         </is>
       </c>
-      <c r="C46" s="9" t="n">
+      <c r="C46" s="10" t="n">
         <v>0.0206</v>
       </c>
-      <c r="D46" s="9" t="n">
+      <c r="D46" s="10" t="n">
         <v>0.0194</v>
       </c>
-      <c r="E46" s="9" t="n">
+      <c r="E46" s="10" t="n">
         <v>0.0212</v>
       </c>
-      <c r="F46" s="9" t="n">
+      <c r="F46" s="10" t="n">
         <v>0.0294</v>
       </c>
-      <c r="G46" s="9" t="inlineStr">
-        <is>
-          <t>mg/L</t>
-        </is>
-      </c>
-      <c r="H46" s="1" t="n"/>
+      <c r="G46" s="10" t="inlineStr">
+        <is>
+          <t>mg/L</t>
+        </is>
+      </c>
+      <c r="H46" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" ht="13" customHeight="1">
+      <c r="A47" s="9" t="inlineStr">
+        <is>
+          <t>Hardness</t>
+        </is>
+      </c>
+      <c r="B47" s="9" t="n"/>
+      <c r="C47" s="10" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="D47" s="10" t="n">
+        <v>23.1</v>
+      </c>
+      <c r="E47" s="10" t="n">
+        <v>22.2</v>
+      </c>
+      <c r="F47" s="10" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="G47" s="1" t="n"/>
+      <c r="H47" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" ht="13" customHeight="1">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>Ph</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="n"/>
+      <c r="C48" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="D48" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="E48" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="F48" s="10" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G48" s="1" t="n"/>
+      <c r="H48" s="6" t="inlineStr">
+        <is>
+          <t>no limit listed</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>